<commit_message>
update gt for user study
</commit_message>
<xml_diff>
--- a/user_study_gt.xlsx
+++ b/user_study_gt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronic\Documents\MSc\Thesis\Projects\TabEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A0C9FC4-6FE5-4202-93F7-3D148CB5C5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEDC72A-3048-45C8-B1E3-1CE756136644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{71915DA3-E129-45EF-ADCC-0CBDFE788319}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{71915DA3-E129-45EF-ADCC-0CBDFE788319}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Cover Type</t>
   </si>
@@ -54,6 +54,27 @@
   </si>
   <si>
     <t>In TabNet the explanations on train are consistent with the test, in VIME not, meaning a good generalization</t>
+  </si>
+  <si>
+    <t>Examples with label 5 are embedded using TabNet based on Soil_Type, closely to each other (the cluster has a significant distribution value of label 5). However, VIME embeddings of these examples are mostly based on Wilderness_Area which splits the labels worse.</t>
+  </si>
+  <si>
+    <t>Examples with label 6 are closely embedded in TabNet based on Elevation mostly, unlike VIME, where they are scattered across all embedding space</t>
+  </si>
+  <si>
+    <t>TabNet captures more complex dividing of the dataset, based on different columns, rather than VIME that splits mostly on a single column</t>
+  </si>
+  <si>
+    <t>TabNet captures more complex dividing of the dataset, based on different columns, rather than VIME that splits based on less columns, therefore its patterns are simpler</t>
+  </si>
+  <si>
+    <t>More insights in the manner of the above</t>
+  </si>
+  <si>
+    <t>Trance examples are embedded using TabNet in separate cluster, whereas using VIME they are embedded in a cluster mixing multiple genres</t>
+  </si>
+  <si>
+    <t>On examples where TabNet outperforms VIME with label Psytrance, it can be seen that VIME confuses psytrance with trance based on their instrumentalness column )have the same range and therefore embeds them closely), where TabNet splits them to different clusters</t>
   </si>
 </sst>
 </file>
@@ -414,17 +435,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C0787A-C389-4344-8A5C-A34221E62F8E}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="131.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="108.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="236.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="150.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -454,6 +475,35 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>